<commit_message>
editteam function bug fix
</commit_message>
<xml_diff>
--- a/team_data/Mumbai_India/Mumbai_India.xlsx
+++ b/team_data/Mumbai_India/Mumbai_India.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IIT\1st Year\1st Trimester\CM1601 [PRO]  Programming Fundamentals\Course Work\team_data\Mumbai_India\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458F2A46-225E-4D8A-8D47-44EEB9D6503F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="6810" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -49,7 +43,7 @@
     <t>Virat Kohli(C)</t>
   </si>
   <si>
-    <t>Pubudu Senarathne</t>
+    <t>Suryakumar Yadav</t>
   </si>
   <si>
     <t>Rishabh Pant</t>
@@ -79,8 +73,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,14 +137,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -197,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,27 +215,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -281,24 +249,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -474,19 +424,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,7 +451,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -526,7 +471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -546,7 +491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -566,7 +511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -586,7 +531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -606,7 +551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -626,7 +571,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -646,7 +591,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -666,7 +611,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -686,7 +631,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -706,7 +651,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
halfway on editing exit button at any stage
</commit_message>
<xml_diff>
--- a/team_data/Mumbai_India/Mumbai_India.xlsx
+++ b/team_data/Mumbai_India/Mumbai_India.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>Player Name</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>Batting Order</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t>KL Rahul</t>
@@ -425,13 +431,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,10 +456,16 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -462,18 +474,21 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -482,18 +497,21 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -502,18 +520,18 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -522,18 +540,18 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -542,18 +560,18 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -562,18 +580,18 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -582,18 +600,18 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -602,18 +620,18 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -622,18 +640,18 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -642,18 +660,18 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -662,10 +680,10 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F12">
         <v>11</v>

</xml_diff>